<commit_message>
Update bug in Colab implementation, add new spectra
</commit_message>
<xml_diff>
--- a/EPSILONINVERSION_FINAL/EpsilonRegression.xlsx
+++ b/EPSILONINVERSION_FINAL/EpsilonRegression.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sarahcshi/Documents/GitHub/BASELINES/EPSILONREGRESSION_FINAL/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sarahcshi/Documents/GitHub/PyIRoGlass/EPSILONINVERSION_FINAL/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{215DD198-4ADB-474F-8221-7FB0F7F375EE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B378BD30-ACC6-6040-ADFB-3B1A05A8138A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="10660" yWindow="500" windowWidth="24220" windowHeight="20800" xr2:uid="{FEE6C955-F107-534A-8F98-4BC8B7F4190E}"/>
+    <workbookView xWindow="11360" yWindow="500" windowWidth="23760" windowHeight="20800" activeTab="3" xr2:uid="{FEE6C955-F107-534A-8F98-4BC8B7F4190E}"/>
   </bookViews>
   <sheets>
     <sheet name="NIRRegress" sheetId="4" r:id="rId1"/>
@@ -1064,7 +1064,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="95">
+  <cellXfs count="104">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1330,6 +1330,27 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="2" fontId="6" fillId="3" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="6" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="6" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="6" fillId="3" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="2" fontId="6" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -1648,8 +1669,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{788A2467-0788-484D-845B-3810F985C6E7}">
   <dimension ref="A1:BS38"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="D7" sqref="D7"/>
+    <sheetView zoomScaleNormal="120" workbookViewId="0">
+      <selection activeCell="B33" sqref="B33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -14852,8 +14873,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{71F3C50D-B1DF-E247-95AB-3AD4B1033E27}">
   <dimension ref="A1:BU33"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E2" sqref="E2"/>
+    <sheetView tabSelected="1" topLeftCell="AU1" workbookViewId="0">
+      <selection activeCell="AW4" sqref="AW4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -15418,7 +15439,7 @@
         <v>1.1674130730136365E-3</v>
       </c>
     </row>
-    <row r="4" spans="1:73" ht="17" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:73" s="95" customFormat="1" ht="17" x14ac:dyDescent="0.25">
       <c r="A4" s="22" t="s">
         <v>47</v>
       </c>
@@ -15480,44 +15501,134 @@
         <v>142</v>
       </c>
       <c r="AI4" s="19"/>
-      <c r="AJ4" s="69"/>
-      <c r="AK4" s="40"/>
-      <c r="AL4" s="40"/>
-      <c r="AM4" s="40"/>
-      <c r="AN4" s="40"/>
-      <c r="AO4" s="40"/>
-      <c r="AP4" s="40"/>
-      <c r="AQ4" s="40"/>
-      <c r="AR4" s="40"/>
+      <c r="AJ4" s="11">
+        <v>47.77</v>
+      </c>
+      <c r="AK4" s="40">
+        <v>0.73</v>
+      </c>
+      <c r="AL4" s="40">
+        <v>15.83</v>
+      </c>
+      <c r="AM4" s="40">
+        <v>8.52</v>
+      </c>
+      <c r="AN4" s="40">
+        <v>0.16</v>
+      </c>
+      <c r="AO4" s="40">
+        <v>10.76</v>
+      </c>
+      <c r="AP4" s="40">
+        <v>11.4</v>
+      </c>
+      <c r="AQ4" s="40">
+        <v>2.2999999999999998</v>
+      </c>
+      <c r="AR4" s="40">
+        <v>0.1</v>
+      </c>
       <c r="AS4" s="40"/>
-      <c r="AT4" s="40"/>
+      <c r="AT4" s="40">
+        <f>SUM(AJ4:AS4)</f>
+        <v>97.57</v>
+      </c>
       <c r="AU4" s="40"/>
-      <c r="AV4" s="40"/>
-      <c r="AW4" s="40"/>
+      <c r="AV4" s="40">
+        <f>(AY4+BA4)/BI4</f>
+        <v>0.59817209210889832</v>
+      </c>
+      <c r="AW4" s="103">
+        <f>BS4/(BS4+BR4)</f>
+        <v>0.26744623595991968</v>
+      </c>
       <c r="AX4" s="40"/>
-      <c r="AY4" s="40"/>
-      <c r="AZ4" s="40"/>
-      <c r="BA4" s="40"/>
-      <c r="BB4" s="40"/>
-      <c r="BC4" s="40"/>
-      <c r="BD4" s="40"/>
-      <c r="BE4" s="40"/>
-      <c r="BF4" s="40"/>
-      <c r="BG4" s="40"/>
-      <c r="BH4" s="40"/>
-      <c r="BI4" s="40"/>
+      <c r="AY4" s="40">
+        <f>AJ4/60.08</f>
+        <v>0.7951065246338217</v>
+      </c>
+      <c r="AZ4" s="40">
+        <f>AK4/79.866</f>
+        <v>9.1403100192822984E-3</v>
+      </c>
+      <c r="BA4" s="40">
+        <f>AL4/101.96</f>
+        <v>0.15525696351510399</v>
+      </c>
+      <c r="BB4" s="40">
+        <f>AM4/71.844</f>
+        <v>0.11859027893769836</v>
+      </c>
+      <c r="BC4" s="40">
+        <f>AN4/70.9374</f>
+        <v>2.2555097875027845E-3</v>
+      </c>
+      <c r="BD4" s="40">
+        <f>AO4/40.3044</f>
+        <v>0.26696837069898072</v>
+      </c>
+      <c r="BE4" s="40">
+        <f>AP4/56.0774</f>
+        <v>0.20329045212509855</v>
+      </c>
+      <c r="BF4" s="40">
+        <f>AQ4/61.9789</f>
+        <v>3.7109403361466557E-2</v>
+      </c>
+      <c r="BG4" s="40">
+        <f>AR4/94.2</f>
+        <v>1.0615711252653928E-3</v>
+      </c>
+      <c r="BH4" s="40">
+        <f>AS4/141.9445</f>
+        <v>0</v>
+      </c>
+      <c r="BI4" s="40">
+        <f>SUM(AY4:BH4)</f>
+        <v>1.5887793842042204</v>
+      </c>
       <c r="BJ4" s="40"/>
       <c r="BK4" s="40"/>
-      <c r="BL4" s="40"/>
-      <c r="BM4" s="40"/>
-      <c r="BN4" s="40"/>
-      <c r="BO4" s="40"/>
-      <c r="BP4" s="40"/>
-      <c r="BQ4" s="40"/>
-      <c r="BR4" s="40"/>
-      <c r="BS4" s="40"/>
-      <c r="BT4" s="40"/>
-      <c r="BU4" s="68"/>
+      <c r="BL4" s="40">
+        <f>AY4</f>
+        <v>0.7951065246338217</v>
+      </c>
+      <c r="BM4" s="40">
+        <f t="shared" ref="BM4:BT4" si="0">AZ4</f>
+        <v>9.1403100192822984E-3</v>
+      </c>
+      <c r="BN4" s="40">
+        <f>BA4*2</f>
+        <v>0.31051392703020797</v>
+      </c>
+      <c r="BO4" s="40">
+        <f t="shared" si="0"/>
+        <v>0.11859027893769836</v>
+      </c>
+      <c r="BP4" s="40">
+        <f t="shared" si="0"/>
+        <v>2.2555097875027845E-3</v>
+      </c>
+      <c r="BQ4" s="40">
+        <f t="shared" si="0"/>
+        <v>0.26696837069898072</v>
+      </c>
+      <c r="BR4" s="40">
+        <f t="shared" si="0"/>
+        <v>0.20329045212509855</v>
+      </c>
+      <c r="BS4" s="40">
+        <f>BF4*2</f>
+        <v>7.4218806722933114E-2</v>
+      </c>
+      <c r="BT4" s="40">
+        <f>BG4*2</f>
+        <v>2.1231422505307855E-3</v>
+      </c>
+      <c r="BU4" s="40">
+        <f>BH4*2</f>
+        <v>0</v>
+      </c>
     </row>
     <row r="5" spans="1:73" ht="17" x14ac:dyDescent="0.25">
       <c r="A5" s="8" t="s">
@@ -18102,182 +18213,182 @@
         <v>0</v>
       </c>
     </row>
-    <row r="20" spans="1:73" s="20" customFormat="1" ht="17" x14ac:dyDescent="0.25">
-      <c r="A20" s="22" t="s">
+    <row r="20" spans="1:73" s="102" customFormat="1" ht="17" x14ac:dyDescent="0.25">
+      <c r="A20" s="96" t="s">
         <v>130</v>
       </c>
-      <c r="B20" s="23" t="s">
+      <c r="B20" s="97" t="s">
         <v>129</v>
       </c>
-      <c r="C20" s="36" t="s">
+      <c r="C20" s="98" t="s">
         <v>128</v>
       </c>
-      <c r="D20" s="36" t="s">
+      <c r="D20" s="98" t="s">
         <v>61</v>
       </c>
-      <c r="E20" s="37" t="s">
+      <c r="E20" s="99" t="s">
         <v>107</v>
       </c>
-      <c r="F20" s="67">
+      <c r="F20" s="12">
         <v>0.622</v>
       </c>
-      <c r="G20" s="67">
+      <c r="G20" s="12">
         <v>0.23157895182099122</v>
       </c>
-      <c r="H20" s="66">
+      <c r="H20" s="11">
         <v>1.02</v>
       </c>
       <c r="I20" s="12">
         <v>0.03</v>
       </c>
-      <c r="J20" s="13"/>
-      <c r="K20" s="65"/>
-      <c r="L20" s="16">
+      <c r="J20" s="12"/>
+      <c r="K20" s="35"/>
+      <c r="L20" s="12">
         <v>0.62</v>
       </c>
-      <c r="M20" s="16">
+      <c r="M20" s="12">
         <v>0.06</v>
       </c>
-      <c r="N20" s="16"/>
-      <c r="O20" s="16"/>
-      <c r="P20" s="15"/>
-      <c r="Q20" s="16"/>
-      <c r="R20" s="18"/>
-      <c r="S20" s="16">
+      <c r="N20" s="12"/>
+      <c r="O20" s="12"/>
+      <c r="P20" s="11"/>
+      <c r="Q20" s="12"/>
+      <c r="R20" s="35"/>
+      <c r="S20" s="12">
         <v>63.9</v>
       </c>
-      <c r="T20" s="16"/>
-      <c r="U20" s="16"/>
-      <c r="V20" s="16"/>
-      <c r="W20" s="16"/>
-      <c r="X20" s="16">
+      <c r="T20" s="12"/>
+      <c r="U20" s="12"/>
+      <c r="V20" s="12"/>
+      <c r="W20" s="12"/>
+      <c r="X20" s="12">
         <v>5.4</v>
       </c>
-      <c r="Y20" s="21"/>
-      <c r="Z20" s="15">
+      <c r="Y20" s="40"/>
+      <c r="Z20" s="11">
         <v>308</v>
       </c>
-      <c r="AA20" s="63" t="s">
+      <c r="AA20" s="68" t="s">
         <v>135</v>
       </c>
-      <c r="AB20" s="15">
+      <c r="AB20" s="11">
         <v>308</v>
       </c>
-      <c r="AC20" s="16">
+      <c r="AC20" s="12">
         <v>110</v>
       </c>
-      <c r="AD20" s="18"/>
-      <c r="AE20" s="16"/>
-      <c r="AF20" s="16"/>
-      <c r="AG20" s="18"/>
-      <c r="AH20" s="57" t="s">
+      <c r="AD20" s="35"/>
+      <c r="AE20" s="12"/>
+      <c r="AF20" s="12"/>
+      <c r="AG20" s="35"/>
+      <c r="AH20" s="100" t="s">
         <v>127</v>
       </c>
-      <c r="AI20" s="57"/>
-      <c r="AJ20" s="64">
+      <c r="AI20" s="100"/>
+      <c r="AJ20" s="101">
         <v>47.645000000000003</v>
       </c>
-      <c r="AK20" s="21">
+      <c r="AK20" s="40">
         <v>0.85750000000000004</v>
       </c>
-      <c r="AL20" s="21">
+      <c r="AL20" s="40">
         <v>14.969999999999999</v>
       </c>
-      <c r="AM20" s="21">
+      <c r="AM20" s="40">
         <v>7.1875</v>
       </c>
-      <c r="AN20" s="21">
+      <c r="AN20" s="40">
         <v>6.5000000000000002E-2</v>
       </c>
-      <c r="AO20" s="21">
+      <c r="AO20" s="40">
         <v>5.4974999999999996</v>
       </c>
-      <c r="AP20" s="21">
+      <c r="AP20" s="40">
         <v>10.82</v>
       </c>
-      <c r="AQ20" s="21">
+      <c r="AQ20" s="40">
         <v>1.7949999999999999</v>
       </c>
-      <c r="AR20" s="21">
+      <c r="AR20" s="40">
         <v>6.902499999999999</v>
       </c>
-      <c r="AS20" s="21">
+      <c r="AS20" s="40">
         <v>0.5</v>
       </c>
-      <c r="AT20" s="59">
+      <c r="AT20" s="40">
         <v>96.24</v>
       </c>
-      <c r="AU20" s="59"/>
-      <c r="AV20" s="21">
+      <c r="AU20" s="40"/>
+      <c r="AV20" s="40">
         <v>0.62682687850579211</v>
       </c>
-      <c r="AW20" s="21">
+      <c r="AW20" s="40">
         <v>0.23157895182099122</v>
       </c>
-      <c r="AX20" s="59"/>
-      <c r="AY20" s="59">
+      <c r="AX20" s="40"/>
+      <c r="AY20" s="40">
         <v>0.79289399234481606</v>
       </c>
-      <c r="AZ20" s="59">
+      <c r="AZ20" s="40">
         <v>1.0732165206508135E-2</v>
       </c>
-      <c r="BA20" s="21">
+      <c r="BA20" s="40">
         <v>0.14682228324833269</v>
       </c>
-      <c r="BB20" s="59">
+      <c r="BB20" s="40">
         <v>0.10003479471120391</v>
       </c>
-      <c r="BC20" s="21">
+      <c r="BC20" s="40">
         <v>9.1626726811389915E-4</v>
       </c>
-      <c r="BD20" s="21">
+      <c r="BD20" s="40">
         <v>0.13638055073182834</v>
       </c>
-      <c r="BE20" s="21">
+      <c r="BE20" s="40">
         <v>0.19293865905848787</v>
       </c>
-      <c r="BF20" s="21">
+      <c r="BF20" s="40">
         <v>2.9045307443365698E-2</v>
       </c>
-      <c r="BG20" s="21">
+      <c r="BG20" s="40">
         <v>7.3274946921443734E-2</v>
       </c>
-      <c r="BH20" s="21">
+      <c r="BH20" s="40">
         <v>8.8059175766114835E-4</v>
       </c>
-      <c r="BI20" s="21">
+      <c r="BI20" s="40">
         <v>1.4839195586917615</v>
       </c>
-      <c r="BJ20" s="59"/>
-      <c r="BK20" s="59"/>
-      <c r="BL20" s="21">
+      <c r="BJ20" s="40"/>
+      <c r="BK20" s="40"/>
+      <c r="BL20" s="40">
         <v>0.79289399234481606</v>
       </c>
-      <c r="BM20" s="21">
+      <c r="BM20" s="40">
         <v>1.0732165206508135E-2</v>
       </c>
-      <c r="BN20" s="21">
+      <c r="BN20" s="40">
         <v>0.29364456649666537</v>
       </c>
-      <c r="BO20" s="21">
+      <c r="BO20" s="40">
         <v>0.10003479471120391</v>
       </c>
-      <c r="BP20" s="21">
+      <c r="BP20" s="40">
         <v>9.1626726811389915E-4</v>
       </c>
-      <c r="BQ20" s="21">
+      <c r="BQ20" s="40">
         <v>0.13638055073182834</v>
       </c>
-      <c r="BR20" s="21">
+      <c r="BR20" s="40">
         <v>0.19293865905848787</v>
       </c>
-      <c r="BS20" s="21">
+      <c r="BS20" s="40">
         <v>5.8090614886731395E-2</v>
       </c>
-      <c r="BT20" s="21">
+      <c r="BT20" s="40">
         <v>0.14654989384288747</v>
       </c>
-      <c r="BU20" s="63">
+      <c r="BU20" s="68">
         <v>1.7611835153222967E-3</v>
       </c>
     </row>

</xml_diff>